<commit_message>
data(megafile): update with XM
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -5805,7 +5805,7 @@
         <v>0.838</v>
       </c>
     </row>
-    <row r="33" spans="1:61">
+    <row r="33" spans="1:65">
       <c r="A33" t="s">
         <v>96</v>
       </c>
@@ -5957,7 +5957,7 @@
         <v>0.8159999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:61">
+    <row r="34" spans="1:65">
       <c r="A34" t="s">
         <v>97</v>
       </c>
@@ -6082,7 +6082,7 @@
         <v>0.452</v>
       </c>
     </row>
-    <row r="35" spans="1:61">
+    <row r="35" spans="1:65">
       <c r="A35" t="s">
         <v>98</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>0.433</v>
       </c>
     </row>
-    <row r="36" spans="1:61">
+    <row r="36" spans="1:65">
       <c r="A36" t="s">
         <v>99</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>0.594</v>
       </c>
     </row>
-    <row r="37" spans="1:61">
+    <row r="37" spans="1:65">
       <c r="A37" t="s">
         <v>100</v>
       </c>
@@ -6424,7 +6424,7 @@
         <v>0.5629999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:61">
+    <row r="38" spans="1:65">
       <c r="A38" t="s">
         <v>101</v>
       </c>
@@ -6594,7 +6594,7 @@
         <v>0.929</v>
       </c>
     </row>
-    <row r="39" spans="1:61">
+    <row r="39" spans="1:65">
       <c r="A39" t="s">
         <v>102</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>0.665</v>
       </c>
     </row>
-    <row r="40" spans="1:61">
+    <row r="40" spans="1:65">
       <c r="A40" t="s">
         <v>103</v>
       </c>
@@ -6784,7 +6784,7 @@
         <v>83.92</v>
       </c>
     </row>
-    <row r="41" spans="1:61">
+    <row r="41" spans="1:65">
       <c r="A41" t="s">
         <v>104</v>
       </c>
@@ -6900,7 +6900,7 @@
         <v>0.397</v>
       </c>
     </row>
-    <row r="42" spans="1:61">
+    <row r="42" spans="1:65">
       <c r="A42" t="s">
         <v>105</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>0.398</v>
       </c>
     </row>
-    <row r="43" spans="1:61">
+    <row r="43" spans="1:65">
       <c r="A43" t="s">
         <v>106</v>
       </c>
@@ -7173,8 +7173,20 @@
       <c r="BI43">
         <v>0.851</v>
       </c>
+      <c r="BJ43">
+        <v>35996.8</v>
+      </c>
+      <c r="BK43">
+        <v>18.03</v>
+      </c>
+      <c r="BL43">
+        <v>-1.5</v>
+      </c>
+      <c r="BM43">
+        <v>1873.627</v>
+      </c>
     </row>
-    <row r="44" spans="1:61">
+    <row r="44" spans="1:65">
       <c r="A44" t="s">
         <v>107</v>
       </c>
@@ -7287,7 +7299,7 @@
         <v>0.761</v>
       </c>
     </row>
-    <row r="45" spans="1:61">
+    <row r="45" spans="1:65">
       <c r="A45" t="s">
         <v>108</v>
       </c>
@@ -7442,7 +7454,7 @@
         <v>0.767</v>
       </c>
     </row>
-    <row r="46" spans="1:61">
+    <row r="46" spans="1:65">
       <c r="A46" t="s">
         <v>109</v>
       </c>
@@ -7564,7 +7576,7 @@
         <v>0.554</v>
       </c>
     </row>
-    <row r="47" spans="1:61">
+    <row r="47" spans="1:65">
       <c r="A47" t="s">
         <v>110</v>
       </c>
@@ -7686,7 +7698,7 @@
         <v>0.574</v>
       </c>
     </row>
-    <row r="48" spans="1:61">
+    <row r="48" spans="1:65">
       <c r="A48" t="s">
         <v>111</v>
       </c>
@@ -7730,7 +7742,7 @@
         <v>76.25</v>
       </c>
     </row>
-    <row r="49" spans="1:61">
+    <row r="49" spans="1:65">
       <c r="A49" t="s">
         <v>112</v>
       </c>
@@ -7882,7 +7894,7 @@
         <v>0.8100000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:61">
+    <row r="50" spans="1:65">
       <c r="A50" t="s">
         <v>113</v>
       </c>
@@ -8025,7 +8037,7 @@
         <v>0.538</v>
       </c>
     </row>
-    <row r="51" spans="1:61">
+    <row r="51" spans="1:65">
       <c r="A51" t="s">
         <v>114</v>
       </c>
@@ -8189,7 +8201,7 @@
         <v>0.851</v>
       </c>
     </row>
-    <row r="52" spans="1:61">
+    <row r="52" spans="1:65">
       <c r="A52" t="s">
         <v>115</v>
       </c>
@@ -8311,7 +8323,7 @@
         <v>0.783</v>
       </c>
     </row>
-    <row r="53" spans="1:61">
+    <row r="53" spans="1:65">
       <c r="A53" t="s">
         <v>116</v>
       </c>
@@ -8373,7 +8385,7 @@
         <v>78.88</v>
       </c>
     </row>
-    <row r="54" spans="1:61">
+    <row r="54" spans="1:65">
       <c r="A54" t="s">
         <v>117</v>
       </c>
@@ -8552,7 +8564,7 @@
         <v>0.887</v>
       </c>
     </row>
-    <row r="55" spans="1:61">
+    <row r="55" spans="1:65">
       <c r="A55" t="s">
         <v>118</v>
       </c>
@@ -8716,7 +8728,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="56" spans="1:61">
+    <row r="56" spans="1:65">
       <c r="A56" t="s">
         <v>119</v>
       </c>
@@ -8832,7 +8844,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="57" spans="1:61">
+    <row r="57" spans="1:65">
       <c r="A57" t="s">
         <v>120</v>
       </c>
@@ -9001,8 +9013,20 @@
       <c r="BI57">
         <v>0.9399999999999999</v>
       </c>
+      <c r="BJ57">
+        <v>-264.6</v>
+      </c>
+      <c r="BK57">
+        <v>-0.27</v>
+      </c>
+      <c r="BL57">
+        <v>4.36</v>
+      </c>
+      <c r="BM57">
+        <v>-45.516</v>
+      </c>
     </row>
-    <row r="58" spans="1:61">
+    <row r="58" spans="1:65">
       <c r="A58" t="s">
         <v>121</v>
       </c>
@@ -9097,7 +9121,7 @@
         <v>0.524</v>
       </c>
     </row>
-    <row r="59" spans="1:61">
+    <row r="59" spans="1:65">
       <c r="A59" t="s">
         <v>122</v>
       </c>
@@ -9201,7 +9225,7 @@
         <v>0.742</v>
       </c>
     </row>
-    <row r="60" spans="1:61">
+    <row r="60" spans="1:65">
       <c r="A60" t="s">
         <v>123</v>
       </c>
@@ -9356,7 +9380,7 @@
         <v>0.756</v>
       </c>
     </row>
-    <row r="61" spans="1:61">
+    <row r="61" spans="1:65">
       <c r="A61" t="s">
         <v>124</v>
       </c>
@@ -9508,7 +9532,7 @@
         <v>0.759</v>
       </c>
     </row>
-    <row r="62" spans="1:61">
+    <row r="62" spans="1:65">
       <c r="A62" t="s">
         <v>125</v>
       </c>
@@ -9633,7 +9657,7 @@
         <v>0.707</v>
       </c>
     </row>
-    <row r="63" spans="1:61">
+    <row r="63" spans="1:65">
       <c r="A63" t="s">
         <v>126</v>
       </c>
@@ -9767,7 +9791,7 @@
         <v>0.673</v>
       </c>
     </row>
-    <row r="64" spans="1:61">
+    <row r="64" spans="1:65">
       <c r="A64" t="s">
         <v>127</v>
       </c>
@@ -9901,7 +9925,7 @@
         <v>0.592</v>
       </c>
     </row>
-    <row r="65" spans="1:61">
+    <row r="65" spans="1:65">
       <c r="A65" t="s">
         <v>128</v>
       </c>
@@ -9996,7 +10020,7 @@
         <v>0.459</v>
       </c>
     </row>
-    <row r="66" spans="1:61">
+    <row r="66" spans="1:65">
       <c r="A66" t="s">
         <v>129</v>
       </c>
@@ -10171,8 +10195,20 @@
       <c r="BI66">
         <v>0.892</v>
       </c>
+      <c r="BJ66">
+        <v>2070.1</v>
+      </c>
+      <c r="BK66">
+        <v>7.42</v>
+      </c>
+      <c r="BL66">
+        <v>13.68</v>
+      </c>
+      <c r="BM66">
+        <v>1562.118</v>
+      </c>
     </row>
-    <row r="67" spans="1:61">
+    <row r="67" spans="1:65">
       <c r="A67" t="s">
         <v>130</v>
       </c>
@@ -10297,7 +10333,7 @@
         <v>0.611</v>
       </c>
     </row>
-    <row r="68" spans="1:61">
+    <row r="68" spans="1:65">
       <c r="A68" t="s">
         <v>131</v>
       </c>
@@ -10452,7 +10488,7 @@
         <v>0.485</v>
       </c>
     </row>
-    <row r="69" spans="1:61">
+    <row r="69" spans="1:65">
       <c r="A69" t="s">
         <v>132</v>
       </c>
@@ -10535,7 +10571,7 @@
         <v>748962983</v>
       </c>
     </row>
-    <row r="70" spans="1:61">
+    <row r="70" spans="1:65">
       <c r="A70" t="s">
         <v>133</v>
       </c>
@@ -10618,7 +10654,7 @@
         <v>447189915</v>
       </c>
     </row>
-    <row r="71" spans="1:61">
+    <row r="71" spans="1:65">
       <c r="A71" t="s">
         <v>134</v>
       </c>
@@ -10671,7 +10707,7 @@
         <v>80.67</v>
       </c>
     </row>
-    <row r="72" spans="1:61">
+    <row r="72" spans="1:65">
       <c r="A72" t="s">
         <v>135</v>
       </c>
@@ -10793,7 +10829,7 @@
         <v>0.743</v>
       </c>
     </row>
-    <row r="73" spans="1:61">
+    <row r="73" spans="1:65">
       <c r="A73" t="s">
         <v>136</v>
       </c>
@@ -10954,7 +10990,7 @@
         <v>0.9379999999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:61">
+    <row r="74" spans="1:65">
       <c r="A74" t="s">
         <v>137</v>
       </c>
@@ -11127,7 +11163,7 @@
         <v>0.901</v>
       </c>
     </row>
-    <row r="75" spans="1:61">
+    <row r="75" spans="1:65">
       <c r="A75" t="s">
         <v>138</v>
       </c>
@@ -11186,7 +11222,7 @@
         <v>77.66</v>
       </c>
     </row>
-    <row r="76" spans="1:61">
+    <row r="76" spans="1:65">
       <c r="A76" t="s">
         <v>139</v>
       </c>
@@ -11323,7 +11359,7 @@
         <v>0.703</v>
       </c>
     </row>
-    <row r="77" spans="1:61">
+    <row r="77" spans="1:65">
       <c r="A77" t="s">
         <v>140</v>
       </c>
@@ -11445,7 +11481,7 @@
         <v>0.496</v>
       </c>
     </row>
-    <row r="78" spans="1:61">
+    <row r="78" spans="1:65">
       <c r="A78" t="s">
         <v>141</v>
       </c>
@@ -11597,7 +11633,7 @@
         <v>0.8120000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:61">
+    <row r="79" spans="1:65">
       <c r="A79" t="s">
         <v>142</v>
       </c>
@@ -11758,7 +11794,7 @@
         <v>0.947</v>
       </c>
     </row>
-    <row r="80" spans="1:61">
+    <row r="80" spans="1:65">
       <c r="A80" t="s">
         <v>143</v>
       </c>
@@ -13784,7 +13820,7 @@
         <v>0.718</v>
       </c>
     </row>
-    <row r="97" spans="1:61">
+    <row r="97" spans="1:65">
       <c r="A97" t="s">
         <v>160</v>
       </c>
@@ -13813,7 +13849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:61">
+    <row r="98" spans="1:65">
       <c r="A98" t="s">
         <v>161</v>
       </c>
@@ -13961,8 +13997,20 @@
       <c r="BI98">
         <v>0.783</v>
       </c>
+      <c r="BJ98">
+        <v>241230.4</v>
+      </c>
+      <c r="BK98">
+        <v>35.01</v>
+      </c>
+      <c r="BL98">
+        <v>35.9</v>
+      </c>
+      <c r="BM98">
+        <v>2837.045</v>
+      </c>
     </row>
-    <row r="99" spans="1:61">
+    <row r="99" spans="1:65">
       <c r="A99" t="s">
         <v>162</v>
       </c>
@@ -14108,7 +14156,7 @@
         <v>0.674</v>
       </c>
     </row>
-    <row r="100" spans="1:61">
+    <row r="100" spans="1:65">
       <c r="A100" t="s">
         <v>163</v>
       </c>
@@ -14284,7 +14332,7 @@
         <v>0.955</v>
       </c>
     </row>
-    <row r="101" spans="1:61">
+    <row r="101" spans="1:65">
       <c r="A101" t="s">
         <v>164</v>
       </c>
@@ -14334,7 +14382,7 @@
         <v>81.40000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:61">
+    <row r="102" spans="1:65">
       <c r="A102" t="s">
         <v>165</v>
       </c>
@@ -14516,7 +14564,7 @@
         <v>0.919</v>
       </c>
     </row>
-    <row r="103" spans="1:61">
+    <row r="103" spans="1:65">
       <c r="A103" t="s">
         <v>166</v>
       </c>
@@ -14692,7 +14740,7 @@
         <v>0.892</v>
       </c>
     </row>
-    <row r="104" spans="1:61">
+    <row r="104" spans="1:65">
       <c r="A104" t="s">
         <v>167</v>
       </c>
@@ -14844,7 +14892,7 @@
         <v>0.734</v>
       </c>
     </row>
-    <row r="105" spans="1:61">
+    <row r="105" spans="1:65">
       <c r="A105" t="s">
         <v>168</v>
       </c>
@@ -14993,7 +15041,7 @@
         <v>0.919</v>
       </c>
     </row>
-    <row r="106" spans="1:61">
+    <row r="106" spans="1:65">
       <c r="A106" t="s">
         <v>169</v>
       </c>
@@ -15034,7 +15082,7 @@
         <v>101073</v>
       </c>
     </row>
-    <row r="107" spans="1:61">
+    <row r="107" spans="1:65">
       <c r="A107" t="s">
         <v>170</v>
       </c>
@@ -15180,7 +15228,7 @@
         <v>0.729</v>
       </c>
     </row>
-    <row r="108" spans="1:61">
+    <row r="108" spans="1:65">
       <c r="A108" t="s">
         <v>171</v>
       </c>
@@ -15308,7 +15356,7 @@
         <v>0.825</v>
       </c>
     </row>
-    <row r="109" spans="1:61">
+    <row r="109" spans="1:65">
       <c r="A109" t="s">
         <v>172</v>
       </c>
@@ -15436,7 +15484,7 @@
         <v>0.601</v>
       </c>
     </row>
-    <row r="110" spans="1:61">
+    <row r="110" spans="1:65">
       <c r="A110" t="s">
         <v>173</v>
       </c>
@@ -15540,7 +15588,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="111" spans="1:61">
+    <row r="111" spans="1:65">
       <c r="A111" t="s">
         <v>174</v>
       </c>
@@ -15659,7 +15707,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="112" spans="1:61">
+    <row r="112" spans="1:65">
       <c r="A112" t="s">
         <v>175</v>
       </c>
@@ -19847,7 +19895,7 @@
         <v>0.602</v>
       </c>
     </row>
-    <row r="145" spans="1:61">
+    <row r="145" spans="1:65">
       <c r="A145" t="s">
         <v>208</v>
       </c>
@@ -20010,8 +20058,20 @@
       <c r="BI145">
         <v>0.944</v>
       </c>
+      <c r="BJ145">
+        <v>20035.1</v>
+      </c>
+      <c r="BK145">
+        <v>7.27</v>
+      </c>
+      <c r="BL145">
+        <v>10.55</v>
+      </c>
+      <c r="BM145">
+        <v>1166.656</v>
+      </c>
     </row>
-    <row r="146" spans="1:61">
+    <row r="146" spans="1:65">
       <c r="A146" t="s">
         <v>209</v>
       </c>
@@ -20070,7 +20130,7 @@
         <v>77.55</v>
       </c>
     </row>
-    <row r="147" spans="1:61">
+    <row r="147" spans="1:65">
       <c r="A147" t="s">
         <v>210</v>
       </c>
@@ -20219,7 +20279,7 @@
         <v>0.931</v>
       </c>
     </row>
-    <row r="148" spans="1:61">
+    <row r="148" spans="1:65">
       <c r="A148" t="s">
         <v>211</v>
       </c>
@@ -20335,7 +20395,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="149" spans="1:61">
+    <row r="149" spans="1:65">
       <c r="A149" t="s">
         <v>212</v>
       </c>
@@ -20457,7 +20517,7 @@
         <v>0.394</v>
       </c>
     </row>
-    <row r="150" spans="1:61">
+    <row r="150" spans="1:65">
       <c r="A150" t="s">
         <v>213</v>
       </c>
@@ -20597,7 +20657,7 @@
         <v>0.539</v>
       </c>
     </row>
-    <row r="151" spans="1:61">
+    <row r="151" spans="1:65">
       <c r="A151" t="s">
         <v>214</v>
       </c>
@@ -20680,7 +20740,7 @@
         <v>596581283</v>
       </c>
     </row>
-    <row r="152" spans="1:61">
+    <row r="152" spans="1:65">
       <c r="A152" t="s">
         <v>215</v>
       </c>
@@ -20802,7 +20862,7 @@
         <v>0.774</v>
       </c>
     </row>
-    <row r="153" spans="1:61">
+    <row r="153" spans="1:65">
       <c r="A153" t="s">
         <v>216</v>
       </c>
@@ -20972,7 +21032,7 @@
         <v>0.957</v>
       </c>
     </row>
-    <row r="154" spans="1:61">
+    <row r="154" spans="1:65">
       <c r="A154" t="s">
         <v>217</v>
       </c>
@@ -21049,7 +21109,7 @@
         <v>43219954</v>
       </c>
     </row>
-    <row r="155" spans="1:61">
+    <row r="155" spans="1:65">
       <c r="A155" t="s">
         <v>218</v>
       </c>
@@ -21171,7 +21231,7 @@
         <v>0.8129999999999999</v>
       </c>
     </row>
-    <row r="156" spans="1:61">
+    <row r="156" spans="1:65">
       <c r="A156" t="s">
         <v>219</v>
       </c>
@@ -21326,7 +21386,7 @@
         <v>0.5570000000000001</v>
       </c>
     </row>
-    <row r="157" spans="1:61">
+    <row r="157" spans="1:65">
       <c r="A157" t="s">
         <v>220</v>
       </c>
@@ -21391,7 +21451,7 @@
         <v>0.826</v>
       </c>
     </row>
-    <row r="158" spans="1:61">
+    <row r="158" spans="1:65">
       <c r="A158" t="s">
         <v>221</v>
       </c>
@@ -21528,7 +21588,7 @@
         <v>0.708</v>
       </c>
     </row>
-    <row r="159" spans="1:61">
+    <row r="159" spans="1:65">
       <c r="A159" t="s">
         <v>222</v>
       </c>
@@ -21677,7 +21737,7 @@
         <v>0.8149999999999999</v>
       </c>
     </row>
-    <row r="160" spans="1:61">
+    <row r="160" spans="1:65">
       <c r="A160" t="s">
         <v>223</v>
       </c>
@@ -21769,7 +21829,7 @@
         <v>0.555</v>
       </c>
     </row>
-    <row r="161" spans="1:61">
+    <row r="161" spans="1:65">
       <c r="A161" t="s">
         <v>224</v>
       </c>
@@ -21921,7 +21981,7 @@
         <v>0.728</v>
       </c>
     </row>
-    <row r="162" spans="1:61">
+    <row r="162" spans="1:65">
       <c r="A162" t="s">
         <v>225</v>
       </c>
@@ -22069,8 +22129,20 @@
       <c r="BI162">
         <v>0.777</v>
       </c>
+      <c r="BJ162">
+        <v>204307.8</v>
+      </c>
+      <c r="BK162">
+        <v>92.01000000000001</v>
+      </c>
+      <c r="BL162">
+        <v>16.3</v>
+      </c>
+      <c r="BM162">
+        <v>6124.442</v>
+      </c>
     </row>
-    <row r="163" spans="1:61">
+    <row r="163" spans="1:65">
       <c r="A163" t="s">
         <v>226</v>
       </c>
@@ -22216,7 +22288,7 @@
         <v>0.718</v>
       </c>
     </row>
-    <row r="164" spans="1:61">
+    <row r="164" spans="1:65">
       <c r="A164" t="s">
         <v>227</v>
       </c>
@@ -22376,8 +22448,20 @@
       <c r="BI164">
         <v>0.88</v>
       </c>
+      <c r="BJ164">
+        <v>117923.5</v>
+      </c>
+      <c r="BK164">
+        <v>15.85</v>
+      </c>
+      <c r="BL164">
+        <v>-2.78</v>
+      </c>
+      <c r="BM164">
+        <v>3119.917</v>
+      </c>
     </row>
-    <row r="165" spans="1:61">
+    <row r="165" spans="1:65">
       <c r="A165" t="s">
         <v>228</v>
       </c>
@@ -22544,7 +22628,7 @@
         <v>0.864</v>
       </c>
     </row>
-    <row r="166" spans="1:61">
+    <row r="166" spans="1:65">
       <c r="A166" t="s">
         <v>229</v>
       </c>
@@ -22675,7 +22759,7 @@
         <v>0.848</v>
       </c>
     </row>
-    <row r="167" spans="1:61">
+    <row r="167" spans="1:65">
       <c r="A167" t="s">
         <v>230</v>
       </c>
@@ -22833,7 +22917,7 @@
         <v>0.828</v>
       </c>
     </row>
-    <row r="168" spans="1:61">
+    <row r="168" spans="1:65">
       <c r="A168" t="s">
         <v>231</v>
       </c>
@@ -22985,7 +23069,7 @@
         <v>0.824</v>
       </c>
     </row>
-    <row r="169" spans="1:61">
+    <row r="169" spans="1:65">
       <c r="A169" t="s">
         <v>232</v>
       </c>
@@ -23134,7 +23218,7 @@
         <v>0.543</v>
       </c>
     </row>
-    <row r="170" spans="1:61">
+    <row r="170" spans="1:65">
       <c r="A170" t="s">
         <v>233</v>
       </c>
@@ -23259,7 +23343,7 @@
         <v>0.779</v>
       </c>
     </row>
-    <row r="171" spans="1:61">
+    <row r="171" spans="1:65">
       <c r="A171" t="s">
         <v>234</v>
       </c>
@@ -23375,7 +23459,7 @@
         <v>0.759</v>
       </c>
     </row>
-    <row r="172" spans="1:61">
+    <row r="172" spans="1:65">
       <c r="A172" t="s">
         <v>235</v>
       </c>
@@ -23485,7 +23569,7 @@
         <v>0.738</v>
       </c>
     </row>
-    <row r="173" spans="1:61">
+    <row r="173" spans="1:65">
       <c r="A173" t="s">
         <v>236</v>
       </c>
@@ -23583,7 +23667,7 @@
         <v>0.715</v>
       </c>
     </row>
-    <row r="174" spans="1:61">
+    <row r="174" spans="1:65">
       <c r="A174" t="s">
         <v>237</v>
       </c>
@@ -23681,7 +23765,7 @@
         <v>84.97</v>
       </c>
     </row>
-    <row r="175" spans="1:61">
+    <row r="175" spans="1:65">
       <c r="A175" t="s">
         <v>238</v>
       </c>
@@ -23797,7 +23881,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="176" spans="1:61">
+    <row r="176" spans="1:65">
       <c r="A176" t="s">
         <v>239</v>
       </c>
@@ -23946,7 +24030,7 @@
         <v>0.854</v>
       </c>
     </row>
-    <row r="177" spans="1:61">
+    <row r="177" spans="1:65">
       <c r="A177" t="s">
         <v>240</v>
       </c>
@@ -24095,7 +24179,7 @@
         <v>0.512</v>
       </c>
     </row>
-    <row r="178" spans="1:61">
+    <row r="178" spans="1:65">
       <c r="A178" t="s">
         <v>241</v>
       </c>
@@ -24262,7 +24346,7 @@
         <v>0.806</v>
       </c>
     </row>
-    <row r="179" spans="1:61">
+    <row r="179" spans="1:65">
       <c r="A179" t="s">
         <v>242</v>
       </c>
@@ -24384,7 +24468,7 @@
         <v>0.796</v>
       </c>
     </row>
-    <row r="180" spans="1:61">
+    <row r="180" spans="1:65">
       <c r="A180" t="s">
         <v>243</v>
       </c>
@@ -24506,7 +24590,7 @@
         <v>0.452</v>
       </c>
     </row>
-    <row r="181" spans="1:61">
+    <row r="181" spans="1:65">
       <c r="A181" t="s">
         <v>244</v>
       </c>
@@ -24661,7 +24745,7 @@
         <v>0.9379999999999999</v>
       </c>
     </row>
-    <row r="182" spans="1:61">
+    <row r="182" spans="1:65">
       <c r="A182" t="s">
         <v>245</v>
       </c>
@@ -24711,7 +24795,7 @@
         <v>78.95</v>
       </c>
     </row>
-    <row r="183" spans="1:61">
+    <row r="183" spans="1:65">
       <c r="A183" t="s">
         <v>246</v>
       </c>
@@ -24881,7 +24965,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="184" spans="1:61">
+    <row r="184" spans="1:65">
       <c r="A184" t="s">
         <v>247</v>
       </c>
@@ -25054,7 +25138,7 @@
         <v>0.917</v>
       </c>
     </row>
-    <row r="185" spans="1:61">
+    <row r="185" spans="1:65">
       <c r="A185" t="s">
         <v>248</v>
       </c>
@@ -25155,7 +25239,7 @@
         <v>0.5669999999999999</v>
       </c>
     </row>
-    <row r="186" spans="1:61">
+    <row r="186" spans="1:65">
       <c r="A186" t="s">
         <v>249</v>
       </c>
@@ -25265,7 +25349,7 @@
         <v>57.4</v>
       </c>
     </row>
-    <row r="187" spans="1:61">
+    <row r="187" spans="1:65">
       <c r="A187" t="s">
         <v>250</v>
       </c>
@@ -25413,8 +25497,20 @@
       <c r="BI187">
         <v>0.709</v>
       </c>
+      <c r="BJ187">
+        <v>224460.5</v>
+      </c>
+      <c r="BK187">
+        <v>23.97</v>
+      </c>
+      <c r="BL187">
+        <v>7.92</v>
+      </c>
+      <c r="BM187">
+        <v>3738.392</v>
+      </c>
     </row>
-    <row r="188" spans="1:61">
+    <row r="188" spans="1:65">
       <c r="A188" t="s">
         <v>251</v>
       </c>
@@ -25497,7 +25593,7 @@
         <v>434260137</v>
       </c>
     </row>
-    <row r="189" spans="1:61">
+    <row r="189" spans="1:65">
       <c r="A189" t="s">
         <v>252</v>
       </c>
@@ -25655,7 +25751,7 @@
         <v>0.916</v>
       </c>
     </row>
-    <row r="190" spans="1:61">
+    <row r="190" spans="1:65">
       <c r="A190" t="s">
         <v>253</v>
       </c>
@@ -25762,7 +25858,7 @@
         <v>0.433</v>
       </c>
     </row>
-    <row r="191" spans="1:61">
+    <row r="191" spans="1:65">
       <c r="A191" t="s">
         <v>254</v>
       </c>
@@ -25938,7 +26034,7 @@
         <v>0.904</v>
       </c>
     </row>
-    <row r="192" spans="1:61">
+    <row r="192" spans="1:65">
       <c r="A192" t="s">
         <v>255</v>
       </c>

</xml_diff>

<commit_message>
data(grapher): add vaccination metrics to internal file
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -2502,10 +2502,10 @@
         <v>0.95</v>
       </c>
       <c r="R5">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="S5">
-        <v>0.247</v>
+        <v>0.314</v>
       </c>
       <c r="AI5">
         <v>11179354</v>
@@ -6505,16 +6505,16 @@
         <v>0.85</v>
       </c>
       <c r="R37">
-        <v>630</v>
+        <v>593</v>
       </c>
       <c r="S37">
-        <v>16.549</v>
+        <v>15.577</v>
       </c>
       <c r="T37">
-        <v>1900</v>
+        <v>1858</v>
       </c>
       <c r="U37">
-        <v>49.911</v>
+        <v>48.808</v>
       </c>
       <c r="Z37">
         <v>96988</v>
@@ -14338,28 +14338,28 @@
         <v>0.58</v>
       </c>
       <c r="R100">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="S100">
-        <v>16.838</v>
+        <v>16.041</v>
       </c>
       <c r="T100">
-        <v>299</v>
+        <v>322</v>
       </c>
       <c r="U100">
-        <v>34.017</v>
+        <v>36.633</v>
       </c>
       <c r="V100">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="W100">
-        <v>9.443</v>
+        <v>9.67</v>
       </c>
       <c r="X100">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="Y100">
-        <v>18.089</v>
+        <v>19.682</v>
       </c>
       <c r="Z100">
         <v>74285</v>
@@ -24156,16 +24156,16 @@
         <v>0.99</v>
       </c>
       <c r="R176">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="S176">
-        <v>40.676</v>
+        <v>41.979</v>
       </c>
       <c r="T176">
-        <v>6764</v>
+        <v>6760</v>
       </c>
       <c r="U176">
-        <v>979.123</v>
+        <v>978.544</v>
       </c>
       <c r="Z176">
         <v>16048</v>
@@ -26535,22 +26535,22 @@
         <v>1.35</v>
       </c>
       <c r="R194">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="S194">
-        <v>11.703</v>
+        <v>12.736</v>
       </c>
       <c r="T194">
-        <v>439</v>
+        <v>469</v>
       </c>
       <c r="U194">
-        <v>50.37</v>
+        <v>53.812</v>
       </c>
       <c r="X194">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="Y194">
-        <v>15.145</v>
+        <v>17.784</v>
       </c>
       <c r="Z194">
         <v>20087</v>
@@ -28661,22 +28661,22 @@
         <v>0.93</v>
       </c>
       <c r="R210">
-        <v>946</v>
+        <v>962</v>
       </c>
       <c r="S210">
-        <v>13.87</v>
+        <v>14.104</v>
       </c>
       <c r="T210">
-        <v>8983</v>
+        <v>9065</v>
       </c>
       <c r="U210">
-        <v>131.702</v>
+        <v>132.904</v>
       </c>
       <c r="X210">
-        <v>7016</v>
+        <v>7028</v>
       </c>
       <c r="Y210">
-        <v>102.863</v>
+        <v>103.039</v>
       </c>
       <c r="Z210">
         <v>871263</v>
@@ -28837,22 +28837,22 @@
         <v>0.96</v>
       </c>
       <c r="R211">
-        <v>12277</v>
+        <v>11927</v>
       </c>
       <c r="S211">
-        <v>36.877</v>
+        <v>35.826</v>
       </c>
       <c r="T211">
-        <v>42945</v>
+        <v>41607</v>
       </c>
       <c r="U211">
-        <v>128.997</v>
+        <v>124.978</v>
       </c>
       <c r="X211">
-        <v>37858</v>
+        <v>37285</v>
       </c>
       <c r="Y211">
-        <v>113.717</v>
+        <v>111.996</v>
       </c>
       <c r="Z211">
         <v>593828</v>

</xml_diff>